<commit_message>
simple daa fields added to improve compatibility with legacy code. Changed some survey responses to be coded in integers instead of strings. fixed codebook output bug. fixed bug in which realround instructions were not displayed in no practice round preceded.
</commit_message>
<xml_diff>
--- a/docs/Session Info.xlsx
+++ b/docs/Session Info.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="24">
   <si>
     <t>Pressure</t>
   </si>
@@ -77,6 +77,24 @@
   <si>
     <t>Gburg #1</t>
   </si>
+  <si>
+    <t>10am</t>
+  </si>
+  <si>
+    <t>1pm</t>
+  </si>
+  <si>
+    <t>4pm</t>
+  </si>
+  <si>
+    <t>4:15pm</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>Sue</t>
+  </si>
 </sst>
 </file>
 
@@ -120,7 +138,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -137,6 +155,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFA4CDFF"/>
         <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -198,7 +222,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="57">
+  <cellStyleXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -256,25 +280,33 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -285,15 +317,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -303,8 +330,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="16" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="20" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="57">
+  <cellStyles count="71">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -333,6 +384,13 @@
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -361,6 +419,13 @@
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -693,7 +758,7 @@
   <dimension ref="B1:Y28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -712,256 +777,264 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:25" ht="16" customHeight="1">
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="18"/>
-      <c r="M1" s="17" t="s">
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="11"/>
+      <c r="M1" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="17"/>
-      <c r="U1" s="17"/>
-      <c r="V1" s="17"/>
-      <c r="W1" s="17"/>
-      <c r="X1" s="17"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="16"/>
+      <c r="X1" s="16"/>
     </row>
     <row r="2" spans="2:25" ht="16" customHeight="1">
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="J2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="19"/>
-      <c r="L2" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="M2" s="13">
-        <v>1</v>
-      </c>
-      <c r="N2" s="13">
+      <c r="K2" s="12"/>
+      <c r="L2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="M2" s="7">
+        <v>1</v>
+      </c>
+      <c r="N2" s="7">
         <v>2</v>
       </c>
-      <c r="O2" s="13">
+      <c r="O2" s="7">
         <v>3</v>
       </c>
-      <c r="P2" s="13">
+      <c r="P2" s="7">
         <v>4</v>
       </c>
-      <c r="Q2" s="13">
+      <c r="Q2" s="7">
         <v>5</v>
       </c>
-      <c r="R2" s="13">
+      <c r="R2" s="7">
         <v>6</v>
       </c>
-      <c r="S2" s="13">
+      <c r="S2" s="7">
         <v>7</v>
       </c>
-      <c r="T2" s="13">
+      <c r="T2" s="7">
         <v>8</v>
       </c>
-      <c r="U2" s="13">
+      <c r="U2" s="7">
         <v>9</v>
       </c>
-      <c r="V2" s="13">
+      <c r="V2" s="7">
         <v>10</v>
       </c>
-      <c r="W2" s="13">
+      <c r="W2" s="7">
         <v>11</v>
       </c>
-      <c r="X2" s="13">
+      <c r="X2" s="7">
         <v>12</v>
       </c>
-      <c r="Y2" s="13" t="s">
+      <c r="Y2" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="2:25" s="2" customFormat="1" ht="16" customHeight="1">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="23">
         <v>42843</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="24">
         <v>0.5</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1">
+      <c r="G3" s="22"/>
+      <c r="H3" s="22">
         <v>3</v>
       </c>
-      <c r="I3" s="1">
-        <v>1</v>
-      </c>
-      <c r="J3" s="1">
+      <c r="I3" s="22">
+        <v>1</v>
+      </c>
+      <c r="J3" s="22">
         <v>2</v>
       </c>
-      <c r="K3" s="20"/>
-      <c r="L3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M3" s="1">
-        <v>0</v>
-      </c>
-      <c r="N3" s="1">
-        <v>60</v>
-      </c>
-      <c r="O3" s="1">
-        <v>60</v>
-      </c>
-      <c r="P3" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="1">
-        <v>60</v>
-      </c>
-      <c r="R3" s="1">
-        <v>60</v>
-      </c>
-      <c r="S3" s="1">
-        <v>0</v>
-      </c>
-      <c r="T3" s="1">
-        <v>60</v>
-      </c>
-      <c r="U3" s="1">
-        <v>60</v>
-      </c>
-      <c r="V3" s="1">
-        <v>0</v>
-      </c>
-      <c r="W3" s="1">
-        <v>60</v>
-      </c>
-      <c r="X3" s="1">
-        <v>60</v>
-      </c>
-      <c r="Y3" s="1"/>
+      <c r="K3" s="25"/>
+      <c r="L3" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="M3" s="22">
+        <v>0</v>
+      </c>
+      <c r="N3" s="22">
+        <v>60</v>
+      </c>
+      <c r="O3" s="22">
+        <v>60</v>
+      </c>
+      <c r="P3" s="22">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="22">
+        <v>60</v>
+      </c>
+      <c r="R3" s="22">
+        <v>60</v>
+      </c>
+      <c r="S3" s="22">
+        <v>0</v>
+      </c>
+      <c r="T3" s="22">
+        <v>60</v>
+      </c>
+      <c r="U3" s="22">
+        <v>60</v>
+      </c>
+      <c r="V3" s="22">
+        <v>0</v>
+      </c>
+      <c r="W3" s="22">
+        <v>60</v>
+      </c>
+      <c r="X3" s="22">
+        <v>60</v>
+      </c>
+      <c r="Y3" s="22"/>
     </row>
     <row r="4" spans="2:25" ht="16" customHeight="1" thickBot="1">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="27">
         <v>42843</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="28">
         <v>0.67708333333333337</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5">
-        <v>1</v>
-      </c>
-      <c r="I4" s="5">
+      <c r="G4" s="26"/>
+      <c r="H4" s="26">
+        <v>1</v>
+      </c>
+      <c r="I4" s="26">
         <v>2</v>
       </c>
-      <c r="J4" s="5">
+      <c r="J4" s="26">
         <v>3</v>
       </c>
-      <c r="K4" s="21"/>
-      <c r="L4" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="M4" s="6">
-        <v>0</v>
-      </c>
-      <c r="N4" s="6">
-        <v>60</v>
-      </c>
-      <c r="O4" s="6">
-        <v>60</v>
-      </c>
-      <c r="P4" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="6">
-        <v>60</v>
-      </c>
-      <c r="R4" s="6">
-        <v>60</v>
-      </c>
-      <c r="S4" s="6">
-        <v>0</v>
-      </c>
-      <c r="T4" s="6">
-        <v>60</v>
-      </c>
-      <c r="U4" s="6">
-        <v>60</v>
-      </c>
-      <c r="V4" s="6">
-        <v>0</v>
-      </c>
-      <c r="W4" s="6">
-        <v>60</v>
-      </c>
-      <c r="X4" s="6">
-        <v>60</v>
-      </c>
-      <c r="Y4" s="5"/>
+      <c r="K4" s="29"/>
+      <c r="L4" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="M4" s="26">
+        <v>0</v>
+      </c>
+      <c r="N4" s="26">
+        <v>60</v>
+      </c>
+      <c r="O4" s="26">
+        <v>60</v>
+      </c>
+      <c r="P4" s="26">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="26">
+        <v>60</v>
+      </c>
+      <c r="R4" s="26">
+        <v>60</v>
+      </c>
+      <c r="S4" s="26">
+        <v>0</v>
+      </c>
+      <c r="T4" s="26">
+        <v>60</v>
+      </c>
+      <c r="U4" s="26">
+        <v>60</v>
+      </c>
+      <c r="V4" s="26">
+        <v>0</v>
+      </c>
+      <c r="W4" s="26">
+        <v>60</v>
+      </c>
+      <c r="X4" s="26">
+        <v>60</v>
+      </c>
+      <c r="Y4" s="26"/>
     </row>
     <row r="5" spans="2:25" ht="16" customHeight="1">
-      <c r="B5" s="7">
-        <v>1</v>
-      </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7" t="s">
+      <c r="B5" s="5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="19">
+        <v>42849</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="15">
+      <c r="F5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="9">
         <v>3</v>
       </c>
-      <c r="I5" s="15">
+      <c r="I5" s="9">
         <v>2</v>
       </c>
-      <c r="J5" s="15">
-        <v>1</v>
-      </c>
-      <c r="K5" s="22"/>
+      <c r="J5" s="9">
+        <v>1</v>
+      </c>
+      <c r="K5" s="13"/>
       <c r="L5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1004,26 +1077,34 @@
       <c r="Y5" s="1"/>
     </row>
     <row r="6" spans="2:25" ht="16" customHeight="1">
-      <c r="B6" s="8">
+      <c r="B6" s="6">
         <v>2</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8" t="s">
+      <c r="C6" s="20">
+        <v>42849</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="16">
+      <c r="F6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="10">
         <v>3</v>
       </c>
-      <c r="I6" s="16">
-        <v>1</v>
-      </c>
-      <c r="J6" s="16">
+      <c r="I6" s="10">
+        <v>1</v>
+      </c>
+      <c r="J6" s="10">
         <v>2</v>
       </c>
-      <c r="K6" s="23"/>
+      <c r="K6" s="14"/>
       <c r="L6" t="s">
         <v>1</v>
       </c>
@@ -1065,26 +1146,32 @@
       </c>
     </row>
     <row r="7" spans="2:25" ht="16" customHeight="1">
-      <c r="B7" s="7">
+      <c r="B7" s="5">
         <v>3</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7" t="s">
+      <c r="C7" s="19">
+        <v>42849</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="15">
-        <v>1</v>
-      </c>
-      <c r="I7" s="15">
+      <c r="F7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="5"/>
+      <c r="H7" s="9">
+        <v>1</v>
+      </c>
+      <c r="I7" s="9">
         <v>2</v>
       </c>
-      <c r="J7" s="15">
+      <c r="J7" s="9">
         <v>3</v>
       </c>
-      <c r="K7" s="22"/>
+      <c r="K7" s="13"/>
       <c r="L7" s="1" t="s">
         <v>0</v>
       </c>
@@ -1127,26 +1214,32 @@
       <c r="Y7" s="1"/>
     </row>
     <row r="8" spans="2:25" ht="16" customHeight="1">
-      <c r="B8" s="8">
+      <c r="B8" s="6">
         <v>4</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8" t="s">
+      <c r="C8" s="20">
+        <v>42850</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="16">
-        <v>1</v>
-      </c>
-      <c r="I8" s="16">
+      <c r="F8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="6"/>
+      <c r="H8" s="10">
+        <v>1</v>
+      </c>
+      <c r="I8" s="10">
         <v>3</v>
       </c>
-      <c r="J8" s="16">
+      <c r="J8" s="10">
         <v>2</v>
       </c>
-      <c r="K8" s="23"/>
+      <c r="K8" s="14"/>
       <c r="L8" t="s">
         <v>1</v>
       </c>
@@ -1188,26 +1281,32 @@
       </c>
     </row>
     <row r="9" spans="2:25" ht="16" customHeight="1">
-      <c r="B9" s="7">
+      <c r="B9" s="5">
         <v>5</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7" t="s">
+      <c r="C9" s="19">
+        <v>42850</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="15">
+      <c r="F9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="5"/>
+      <c r="H9" s="9">
         <v>2</v>
       </c>
-      <c r="I9" s="15">
-        <v>1</v>
-      </c>
-      <c r="J9" s="15">
+      <c r="I9" s="9">
+        <v>1</v>
+      </c>
+      <c r="J9" s="9">
         <v>3</v>
       </c>
-      <c r="K9" s="22"/>
+      <c r="K9" s="13"/>
       <c r="L9" s="1" t="s">
         <v>0</v>
       </c>
@@ -1250,26 +1349,32 @@
       <c r="Y9" s="1"/>
     </row>
     <row r="10" spans="2:25" ht="16" customHeight="1">
-      <c r="B10" s="8">
+      <c r="B10" s="6">
         <v>6</v>
       </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8" t="s">
+      <c r="C10" s="20">
+        <v>42850</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="16">
+      <c r="F10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="6"/>
+      <c r="H10" s="10">
         <v>2</v>
       </c>
-      <c r="I10" s="16">
+      <c r="I10" s="10">
         <v>3</v>
       </c>
-      <c r="J10" s="16">
-        <v>1</v>
-      </c>
-      <c r="K10" s="23"/>
+      <c r="J10" s="10">
+        <v>1</v>
+      </c>
+      <c r="K10" s="14"/>
       <c r="L10" t="s">
         <v>1</v>
       </c>
@@ -1311,26 +1416,32 @@
       </c>
     </row>
     <row r="11" spans="2:25" ht="16" customHeight="1">
-      <c r="B11" s="7">
+      <c r="B11" s="5">
         <v>7</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7" t="s">
+      <c r="C11" s="19">
+        <v>42851</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="15">
+      <c r="F11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="5"/>
+      <c r="H11" s="9">
         <v>2</v>
       </c>
-      <c r="I11" s="15">
+      <c r="I11" s="9">
         <v>3</v>
       </c>
-      <c r="J11" s="15">
-        <v>1</v>
-      </c>
-      <c r="K11" s="22"/>
+      <c r="J11" s="9">
+        <v>1</v>
+      </c>
+      <c r="K11" s="13"/>
       <c r="L11" s="1" t="s">
         <v>0</v>
       </c>
@@ -1373,26 +1484,32 @@
       <c r="Y11" s="1"/>
     </row>
     <row r="12" spans="2:25" ht="16" customHeight="1">
-      <c r="B12" s="8">
+      <c r="B12" s="6">
         <v>8</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8" t="s">
+      <c r="C12" s="20">
+        <v>42851</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="16">
+      <c r="F12" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="6"/>
+      <c r="H12" s="10">
         <v>2</v>
       </c>
-      <c r="I12" s="16">
-        <v>1</v>
-      </c>
-      <c r="J12" s="16">
+      <c r="I12" s="10">
+        <v>1</v>
+      </c>
+      <c r="J12" s="10">
         <v>3</v>
       </c>
-      <c r="K12" s="23"/>
+      <c r="K12" s="14"/>
       <c r="L12" t="s">
         <v>1</v>
       </c>
@@ -1434,26 +1551,32 @@
       </c>
     </row>
     <row r="13" spans="2:25" ht="16" customHeight="1">
-      <c r="B13" s="7">
+      <c r="B13" s="5">
         <v>9</v>
       </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7" t="s">
+      <c r="C13" s="19">
+        <v>42851</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="15">
-        <v>1</v>
-      </c>
-      <c r="I13" s="15">
+      <c r="F13" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" s="5"/>
+      <c r="H13" s="9">
+        <v>1</v>
+      </c>
+      <c r="I13" s="9">
         <v>3</v>
       </c>
-      <c r="J13" s="15">
+      <c r="J13" s="9">
         <v>2</v>
       </c>
-      <c r="K13" s="22"/>
+      <c r="K13" s="13"/>
       <c r="L13" s="1" t="s">
         <v>0</v>
       </c>
@@ -1496,26 +1619,32 @@
       <c r="Y13" s="1"/>
     </row>
     <row r="14" spans="2:25" ht="16" customHeight="1">
-      <c r="B14" s="8">
+      <c r="B14" s="6">
         <v>10</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="16">
-        <v>1</v>
-      </c>
-      <c r="I14" s="16">
+      <c r="C14" s="20">
+        <v>42852</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" s="6"/>
+      <c r="H14" s="10">
+        <v>1</v>
+      </c>
+      <c r="I14" s="10">
         <v>2</v>
       </c>
-      <c r="J14" s="16">
+      <c r="J14" s="10">
         <v>3</v>
       </c>
-      <c r="K14" s="23"/>
+      <c r="K14" s="14"/>
       <c r="L14" t="s">
         <v>1</v>
       </c>
@@ -1557,26 +1686,32 @@
       </c>
     </row>
     <row r="15" spans="2:25" ht="16" customHeight="1">
-      <c r="B15" s="7">
+      <c r="B15" s="5">
         <v>11</v>
       </c>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="15">
+      <c r="C15" s="19">
+        <v>42852</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" s="5"/>
+      <c r="H15" s="9">
         <v>3</v>
       </c>
-      <c r="I15" s="15">
-        <v>1</v>
-      </c>
-      <c r="J15" s="15">
+      <c r="I15" s="9">
+        <v>1</v>
+      </c>
+      <c r="J15" s="9">
         <v>2</v>
       </c>
-      <c r="K15" s="22"/>
+      <c r="K15" s="13"/>
       <c r="L15" s="1" t="s">
         <v>0</v>
       </c>
@@ -1622,78 +1757,75 @@
       <c r="B16" s="8">
         <v>12</v>
       </c>
-      <c r="C16" s="8"/>
+      <c r="C16" s="21"/>
       <c r="D16" s="8"/>
-      <c r="E16" s="8" t="s">
-        <v>6</v>
-      </c>
+      <c r="E16" s="8"/>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
-      <c r="H16" s="16">
+      <c r="H16" s="17">
         <v>3</v>
       </c>
-      <c r="I16" s="16">
+      <c r="I16" s="17">
         <v>2</v>
       </c>
-      <c r="J16" s="16">
-        <v>1</v>
-      </c>
-      <c r="K16" s="23"/>
-      <c r="L16" t="s">
-        <v>1</v>
-      </c>
-      <c r="M16" s="2">
-        <v>60</v>
-      </c>
-      <c r="N16" s="2">
-        <v>60</v>
-      </c>
-      <c r="O16" s="2">
-        <v>60</v>
-      </c>
-      <c r="P16" s="2">
-        <v>60</v>
-      </c>
-      <c r="Q16" s="2">
-        <v>0</v>
-      </c>
-      <c r="R16" s="2">
-        <v>0</v>
-      </c>
-      <c r="S16" s="2">
-        <v>60</v>
-      </c>
-      <c r="T16" s="2">
-        <v>60</v>
-      </c>
-      <c r="U16" s="2">
-        <v>60</v>
-      </c>
-      <c r="V16" s="2">
-        <v>60</v>
-      </c>
-      <c r="W16" s="2">
-        <v>0</v>
-      </c>
-      <c r="X16" s="2">
-        <v>0</v>
-      </c>
+      <c r="J16" s="17">
+        <v>1</v>
+      </c>
+      <c r="K16" s="15"/>
+      <c r="L16" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="M16" s="18">
+        <v>60</v>
+      </c>
+      <c r="N16" s="18">
+        <v>60</v>
+      </c>
+      <c r="O16" s="18">
+        <v>60</v>
+      </c>
+      <c r="P16" s="18">
+        <v>60</v>
+      </c>
+      <c r="Q16" s="18">
+        <v>0</v>
+      </c>
+      <c r="R16" s="18">
+        <v>0</v>
+      </c>
+      <c r="S16" s="18">
+        <v>60</v>
+      </c>
+      <c r="T16" s="18">
+        <v>60</v>
+      </c>
+      <c r="U16" s="18">
+        <v>60</v>
+      </c>
+      <c r="V16" s="18">
+        <v>60</v>
+      </c>
+      <c r="W16" s="18">
+        <v>0</v>
+      </c>
+      <c r="X16" s="18">
+        <v>0</v>
+      </c>
+      <c r="Y16" s="7"/>
     </row>
     <row r="17" spans="2:25" ht="16" customHeight="1">
-      <c r="B17" s="7">
+      <c r="B17" s="5">
         <v>13</v>
       </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="22"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="13"/>
       <c r="L17" s="1" t="s">
         <v>0</v>
       </c>
@@ -1736,20 +1868,18 @@
       <c r="Y17" s="1"/>
     </row>
     <row r="18" spans="2:25" ht="16" customHeight="1">
-      <c r="B18" s="8">
+      <c r="B18" s="6">
         <v>14</v>
       </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="23"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="14"/>
       <c r="L18" t="s">
         <v>1</v>
       </c>
@@ -1791,20 +1921,18 @@
       </c>
     </row>
     <row r="19" spans="2:25" ht="16" customHeight="1">
-      <c r="B19" s="7">
+      <c r="B19" s="5">
         <v>15</v>
       </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="22"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="13"/>
       <c r="L19" s="1" t="s">
         <v>0</v>
       </c>
@@ -1847,20 +1975,18 @@
       <c r="Y19" s="1"/>
     </row>
     <row r="20" spans="2:25" ht="16" customHeight="1">
-      <c r="B20" s="8">
+      <c r="B20" s="6">
         <v>16</v>
       </c>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="23"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="14"/>
       <c r="L20" t="s">
         <v>1</v>
       </c>
@@ -1902,20 +2028,18 @@
       </c>
     </row>
     <row r="21" spans="2:25" ht="16" customHeight="1">
-      <c r="B21" s="7">
+      <c r="B21" s="5">
         <v>17</v>
       </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="22"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="13"/>
       <c r="L21" s="1" t="s">
         <v>0</v>
       </c>
@@ -1963,220 +2087,375 @@
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
-      <c r="E22" s="8" t="s">
-        <v>6</v>
-      </c>
+      <c r="E22" s="8"/>
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="23"/>
-      <c r="L22" t="s">
-        <v>1</v>
-      </c>
-      <c r="M22" s="2">
-        <v>60</v>
-      </c>
-      <c r="N22" s="2">
-        <v>60</v>
-      </c>
-      <c r="O22" s="2">
-        <v>60</v>
-      </c>
-      <c r="P22" s="2">
-        <v>60</v>
-      </c>
-      <c r="Q22" s="2">
-        <v>60</v>
-      </c>
-      <c r="R22" s="2">
-        <v>60</v>
-      </c>
-      <c r="S22" s="2">
-        <v>60</v>
-      </c>
-      <c r="T22" s="2">
-        <v>60</v>
-      </c>
-      <c r="U22" s="2">
-        <v>0</v>
-      </c>
-      <c r="V22" s="2">
-        <v>0</v>
-      </c>
-      <c r="W22" s="2">
-        <v>0</v>
-      </c>
-      <c r="X22" s="2">
-        <v>0</v>
-      </c>
+      <c r="H22" s="17"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="17"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="M22" s="18">
+        <v>60</v>
+      </c>
+      <c r="N22" s="18">
+        <v>60</v>
+      </c>
+      <c r="O22" s="18">
+        <v>60</v>
+      </c>
+      <c r="P22" s="18">
+        <v>60</v>
+      </c>
+      <c r="Q22" s="18">
+        <v>60</v>
+      </c>
+      <c r="R22" s="18">
+        <v>60</v>
+      </c>
+      <c r="S22" s="18">
+        <v>60</v>
+      </c>
+      <c r="T22" s="18">
+        <v>60</v>
+      </c>
+      <c r="U22" s="18">
+        <v>0</v>
+      </c>
+      <c r="V22" s="18">
+        <v>0</v>
+      </c>
+      <c r="W22" s="18">
+        <v>0</v>
+      </c>
+      <c r="X22" s="18">
+        <v>0</v>
+      </c>
+      <c r="Y22" s="7"/>
     </row>
     <row r="23" spans="2:25" ht="16" customHeight="1">
-      <c r="B23" s="7">
+      <c r="B23" s="5">
         <v>19</v>
       </c>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="22"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="13"/>
       <c r="L23" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
-      <c r="O23" s="1"/>
-      <c r="P23" s="1"/>
-      <c r="Q23" s="1"/>
-      <c r="R23" s="1"/>
-      <c r="S23" s="1"/>
-      <c r="T23" s="1"/>
-      <c r="U23" s="1"/>
-      <c r="V23" s="1"/>
-      <c r="W23" s="1"/>
-      <c r="X23" s="1"/>
+      <c r="M23" s="1">
+        <v>0</v>
+      </c>
+      <c r="N23" s="1">
+        <v>60</v>
+      </c>
+      <c r="O23" s="1">
+        <v>60</v>
+      </c>
+      <c r="P23" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="1">
+        <v>60</v>
+      </c>
+      <c r="R23" s="1">
+        <v>60</v>
+      </c>
+      <c r="S23" s="1">
+        <v>0</v>
+      </c>
+      <c r="T23" s="1">
+        <v>60</v>
+      </c>
+      <c r="U23" s="1">
+        <v>60</v>
+      </c>
+      <c r="V23" s="1">
+        <v>0</v>
+      </c>
+      <c r="W23" s="1">
+        <v>60</v>
+      </c>
+      <c r="X23" s="1">
+        <v>60</v>
+      </c>
       <c r="Y23" s="1"/>
     </row>
     <row r="24" spans="2:25" ht="16" customHeight="1">
-      <c r="B24" s="8">
+      <c r="B24" s="6">
         <v>20</v>
       </c>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="23"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="14"/>
       <c r="L24" t="s">
         <v>1</v>
       </c>
+      <c r="M24" s="2">
+        <v>0</v>
+      </c>
+      <c r="N24" s="2">
+        <v>60</v>
+      </c>
+      <c r="O24" s="2">
+        <v>60</v>
+      </c>
+      <c r="P24" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="2">
+        <v>60</v>
+      </c>
+      <c r="R24" s="2">
+        <v>60</v>
+      </c>
+      <c r="S24" s="2">
+        <v>0</v>
+      </c>
+      <c r="T24" s="2">
+        <v>60</v>
+      </c>
+      <c r="U24" s="2">
+        <v>60</v>
+      </c>
+      <c r="V24" s="2">
+        <v>0</v>
+      </c>
+      <c r="W24" s="2">
+        <v>60</v>
+      </c>
+      <c r="X24" s="2">
+        <v>60</v>
+      </c>
     </row>
     <row r="25" spans="2:25" ht="16" customHeight="1">
-      <c r="B25" s="7">
+      <c r="B25" s="5">
         <v>21</v>
       </c>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="7"/>
-      <c r="K25" s="22"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="13"/>
       <c r="L25" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
-      <c r="O25" s="1"/>
-      <c r="P25" s="1"/>
-      <c r="Q25" s="1"/>
-      <c r="R25" s="1"/>
-      <c r="S25" s="1"/>
-      <c r="T25" s="1"/>
-      <c r="U25" s="1"/>
-      <c r="V25" s="1"/>
-      <c r="W25" s="1"/>
-      <c r="X25" s="1"/>
+      <c r="M25" s="1">
+        <v>60</v>
+      </c>
+      <c r="N25" s="1">
+        <v>0</v>
+      </c>
+      <c r="O25" s="3">
+        <v>60</v>
+      </c>
+      <c r="P25" s="1">
+        <v>60</v>
+      </c>
+      <c r="Q25" s="1">
+        <v>0</v>
+      </c>
+      <c r="R25" s="3">
+        <v>60</v>
+      </c>
+      <c r="S25" s="1">
+        <v>60</v>
+      </c>
+      <c r="T25" s="1">
+        <v>0</v>
+      </c>
+      <c r="U25" s="3">
+        <v>60</v>
+      </c>
+      <c r="V25" s="1">
+        <v>60</v>
+      </c>
+      <c r="W25" s="1">
+        <v>0</v>
+      </c>
+      <c r="X25" s="3">
+        <v>60</v>
+      </c>
       <c r="Y25" s="1"/>
     </row>
     <row r="26" spans="2:25" ht="16" customHeight="1">
-      <c r="B26" s="8">
+      <c r="B26" s="6">
         <v>22</v>
       </c>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
-      <c r="K26" s="23"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="14"/>
       <c r="L26" t="s">
         <v>1</v>
       </c>
+      <c r="M26" s="2">
+        <v>60</v>
+      </c>
+      <c r="N26" s="2">
+        <v>0</v>
+      </c>
+      <c r="O26" s="4">
+        <v>60</v>
+      </c>
+      <c r="P26" s="2">
+        <v>60</v>
+      </c>
+      <c r="Q26" s="2">
+        <v>0</v>
+      </c>
+      <c r="R26" s="4">
+        <v>60</v>
+      </c>
+      <c r="S26" s="2">
+        <v>60</v>
+      </c>
+      <c r="T26" s="2">
+        <v>0</v>
+      </c>
+      <c r="U26" s="4">
+        <v>60</v>
+      </c>
+      <c r="V26" s="2">
+        <v>60</v>
+      </c>
+      <c r="W26" s="2">
+        <v>0</v>
+      </c>
+      <c r="X26" s="4">
+        <v>60</v>
+      </c>
     </row>
     <row r="27" spans="2:25" ht="16" customHeight="1">
-      <c r="B27" s="7">
+      <c r="B27" s="5">
         <v>23</v>
       </c>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
-      <c r="J27" s="7"/>
-      <c r="K27" s="22"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="13"/>
       <c r="L27" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="M27" s="1"/>
-      <c r="N27" s="1"/>
-      <c r="O27" s="1"/>
-      <c r="P27" s="1"/>
-      <c r="Q27" s="1"/>
-      <c r="R27" s="1"/>
-      <c r="S27" s="1"/>
-      <c r="T27" s="1"/>
-      <c r="U27" s="1"/>
-      <c r="V27" s="1"/>
-      <c r="W27" s="1"/>
-      <c r="X27" s="1"/>
+      <c r="M27" s="3">
+        <v>60</v>
+      </c>
+      <c r="N27" s="1">
+        <v>60</v>
+      </c>
+      <c r="O27" s="1">
+        <v>0</v>
+      </c>
+      <c r="P27" s="3">
+        <v>60</v>
+      </c>
+      <c r="Q27" s="3">
+        <v>60</v>
+      </c>
+      <c r="R27" s="1">
+        <v>0</v>
+      </c>
+      <c r="S27" s="3">
+        <v>60</v>
+      </c>
+      <c r="T27" s="3">
+        <v>60</v>
+      </c>
+      <c r="U27" s="1">
+        <v>0</v>
+      </c>
+      <c r="V27" s="3">
+        <v>60</v>
+      </c>
+      <c r="W27" s="3">
+        <v>60</v>
+      </c>
+      <c r="X27" s="1">
+        <v>0</v>
+      </c>
       <c r="Y27" s="1"/>
     </row>
     <row r="28" spans="2:25" ht="16" customHeight="1">
-      <c r="B28" s="14">
+      <c r="B28" s="8">
         <v>24</v>
       </c>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="14"/>
-      <c r="J28" s="14"/>
-      <c r="K28" s="24"/>
-      <c r="L28" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="M28" s="13"/>
-      <c r="N28" s="13"/>
-      <c r="O28" s="13"/>
-      <c r="P28" s="13"/>
-      <c r="Q28" s="13"/>
-      <c r="R28" s="13"/>
-      <c r="S28" s="13"/>
-      <c r="T28" s="13"/>
-      <c r="U28" s="13"/>
-      <c r="V28" s="13"/>
-      <c r="W28" s="13"/>
-      <c r="X28" s="13"/>
-      <c r="Y28" s="13"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="15"/>
+      <c r="L28" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="M28" s="4">
+        <v>60</v>
+      </c>
+      <c r="N28" s="2">
+        <v>60</v>
+      </c>
+      <c r="O28" s="2">
+        <v>0</v>
+      </c>
+      <c r="P28" s="4">
+        <v>60</v>
+      </c>
+      <c r="Q28" s="4">
+        <v>60</v>
+      </c>
+      <c r="R28" s="2">
+        <v>0</v>
+      </c>
+      <c r="S28" s="4">
+        <v>60</v>
+      </c>
+      <c r="T28" s="4">
+        <v>60</v>
+      </c>
+      <c r="U28" s="2">
+        <v>0</v>
+      </c>
+      <c r="V28" s="4">
+        <v>60</v>
+      </c>
+      <c r="W28" s="4">
+        <v>60</v>
+      </c>
+      <c r="X28" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y28" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Updated Session 1 and 2 on Session Info.xlsx to switch timing conditions for participants 1 and 2
</commit_message>
<xml_diff>
--- a/docs/Session Info.xlsx
+++ b/docs/Session Info.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$1:$X$28</definedName>
   </definedNames>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -330,9 +330,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -354,6 +351,9 @@
     <xf numFmtId="16" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="71">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -430,6 +430,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -758,47 +763,47 @@
   <dimension ref="B1:Y28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" customWidth="1"/>
-    <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.375" customWidth="1"/>
+    <col min="2" max="2" width="7.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="7.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.625" bestFit="1" customWidth="1"/>
     <col min="8" max="10" width="5" customWidth="1"/>
-    <col min="11" max="11" width="1.83203125" customWidth="1"/>
+    <col min="11" max="11" width="1.875" customWidth="1"/>
     <col min="12" max="12" width="10" customWidth="1"/>
     <col min="13" max="24" width="3.5" customWidth="1"/>
-    <col min="25" max="25" width="64.83203125" customWidth="1"/>
+    <col min="25" max="25" width="64.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:25" ht="16" customHeight="1">
-      <c r="H1" s="16" t="s">
+    <row r="1" spans="2:25" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H1" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
       <c r="K1" s="11"/>
-      <c r="M1" s="16" t="s">
+      <c r="M1" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="16"/>
-      <c r="S1" s="16"/>
-      <c r="T1" s="16"/>
-      <c r="U1" s="16"/>
-      <c r="V1" s="16"/>
-      <c r="W1" s="16"/>
-      <c r="X1" s="16"/>
-    </row>
-    <row r="2" spans="2:25" ht="16" customHeight="1">
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="29"/>
+      <c r="V1" s="29"/>
+      <c r="W1" s="29"/>
+      <c r="X1" s="29"/>
+    </row>
+    <row r="2" spans="2:25" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
         <v>9</v>
       </c>
@@ -870,147 +875,147 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="2:25" s="2" customFormat="1" ht="16" customHeight="1">
-      <c r="B3" s="22" t="s">
+    <row r="3" spans="2:25" s="2" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="23">
+      <c r="C3" s="22">
         <v>42843</v>
       </c>
-      <c r="D3" s="24">
+      <c r="D3" s="23">
         <v>0.5</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22">
+      <c r="G3" s="21"/>
+      <c r="H3" s="21">
         <v>3</v>
       </c>
-      <c r="I3" s="22">
-        <v>1</v>
-      </c>
-      <c r="J3" s="22">
+      <c r="I3" s="21">
+        <v>1</v>
+      </c>
+      <c r="J3" s="21">
         <v>2</v>
       </c>
-      <c r="K3" s="25"/>
-      <c r="L3" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="M3" s="22">
-        <v>0</v>
-      </c>
-      <c r="N3" s="22">
-        <v>60</v>
-      </c>
-      <c r="O3" s="22">
-        <v>60</v>
-      </c>
-      <c r="P3" s="22">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="22">
-        <v>60</v>
-      </c>
-      <c r="R3" s="22">
-        <v>60</v>
-      </c>
-      <c r="S3" s="22">
-        <v>0</v>
-      </c>
-      <c r="T3" s="22">
-        <v>60</v>
-      </c>
-      <c r="U3" s="22">
-        <v>60</v>
-      </c>
-      <c r="V3" s="22">
-        <v>0</v>
-      </c>
-      <c r="W3" s="22">
-        <v>60</v>
-      </c>
-      <c r="X3" s="22">
-        <v>60</v>
-      </c>
-      <c r="Y3" s="22"/>
-    </row>
-    <row r="4" spans="2:25" ht="16" customHeight="1" thickBot="1">
-      <c r="B4" s="26" t="s">
+      <c r="K3" s="24"/>
+      <c r="L3" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="M3" s="21">
+        <v>0</v>
+      </c>
+      <c r="N3" s="21">
+        <v>60</v>
+      </c>
+      <c r="O3" s="21">
+        <v>60</v>
+      </c>
+      <c r="P3" s="21">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="21">
+        <v>60</v>
+      </c>
+      <c r="R3" s="21">
+        <v>60</v>
+      </c>
+      <c r="S3" s="21">
+        <v>0</v>
+      </c>
+      <c r="T3" s="21">
+        <v>60</v>
+      </c>
+      <c r="U3" s="21">
+        <v>60</v>
+      </c>
+      <c r="V3" s="21">
+        <v>0</v>
+      </c>
+      <c r="W3" s="21">
+        <v>60</v>
+      </c>
+      <c r="X3" s="21">
+        <v>60</v>
+      </c>
+      <c r="Y3" s="21"/>
+    </row>
+    <row r="4" spans="2:25" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="27">
+      <c r="C4" s="26">
         <v>42843</v>
       </c>
-      <c r="D4" s="28">
+      <c r="D4" s="27">
         <v>0.67708333333333337</v>
       </c>
-      <c r="E4" s="26" t="s">
+      <c r="E4" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="26" t="s">
+      <c r="F4" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26">
-        <v>1</v>
-      </c>
-      <c r="I4" s="26">
+      <c r="G4" s="25"/>
+      <c r="H4" s="25">
+        <v>1</v>
+      </c>
+      <c r="I4" s="25">
         <v>2</v>
       </c>
-      <c r="J4" s="26">
+      <c r="J4" s="25">
         <v>3</v>
       </c>
-      <c r="K4" s="29"/>
-      <c r="L4" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="M4" s="26">
-        <v>0</v>
-      </c>
-      <c r="N4" s="26">
-        <v>60</v>
-      </c>
-      <c r="O4" s="26">
-        <v>60</v>
-      </c>
-      <c r="P4" s="26">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="26">
-        <v>60</v>
-      </c>
-      <c r="R4" s="26">
-        <v>60</v>
-      </c>
-      <c r="S4" s="26">
-        <v>0</v>
-      </c>
-      <c r="T4" s="26">
-        <v>60</v>
-      </c>
-      <c r="U4" s="26">
-        <v>60</v>
-      </c>
-      <c r="V4" s="26">
-        <v>0</v>
-      </c>
-      <c r="W4" s="26">
-        <v>60</v>
-      </c>
-      <c r="X4" s="26">
-        <v>60</v>
-      </c>
-      <c r="Y4" s="26"/>
-    </row>
-    <row r="5" spans="2:25" ht="16" customHeight="1">
+      <c r="K4" s="28"/>
+      <c r="L4" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="M4" s="25">
+        <v>0</v>
+      </c>
+      <c r="N4" s="25">
+        <v>60</v>
+      </c>
+      <c r="O4" s="25">
+        <v>60</v>
+      </c>
+      <c r="P4" s="25">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="25">
+        <v>60</v>
+      </c>
+      <c r="R4" s="25">
+        <v>60</v>
+      </c>
+      <c r="S4" s="25">
+        <v>0</v>
+      </c>
+      <c r="T4" s="25">
+        <v>60</v>
+      </c>
+      <c r="U4" s="25">
+        <v>60</v>
+      </c>
+      <c r="V4" s="25">
+        <v>0</v>
+      </c>
+      <c r="W4" s="25">
+        <v>60</v>
+      </c>
+      <c r="X4" s="25">
+        <v>60</v>
+      </c>
+      <c r="Y4" s="25"/>
+    </row>
+    <row r="5" spans="2:25" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="5">
         <v>1</v>
       </c>
-      <c r="C5" s="19">
+      <c r="C5" s="18">
         <v>42849</v>
       </c>
       <c r="D5" s="5" t="s">
@@ -1039,10 +1044,10 @@
         <v>0</v>
       </c>
       <c r="M5" s="1">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="N5" s="1">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="O5" s="1">
         <v>60</v>
@@ -1076,11 +1081,11 @@
       </c>
       <c r="Y5" s="1"/>
     </row>
-    <row r="6" spans="2:25" ht="16" customHeight="1">
+    <row r="6" spans="2:25" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="6">
         <v>2</v>
       </c>
-      <c r="C6" s="20">
+      <c r="C6" s="19">
         <v>42849</v>
       </c>
       <c r="D6" s="6" t="s">
@@ -1109,10 +1114,10 @@
         <v>1</v>
       </c>
       <c r="M6" s="2">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="N6" s="2">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="O6" s="2">
         <v>60</v>
@@ -1145,11 +1150,11 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="2:25" ht="16" customHeight="1">
+    <row r="7" spans="2:25" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5">
         <v>3</v>
       </c>
-      <c r="C7" s="19">
+      <c r="C7" s="18">
         <v>42849</v>
       </c>
       <c r="D7" s="5" t="s">
@@ -1213,11 +1218,11 @@
       </c>
       <c r="Y7" s="1"/>
     </row>
-    <row r="8" spans="2:25" ht="16" customHeight="1">
+    <row r="8" spans="2:25" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="6">
         <v>4</v>
       </c>
-      <c r="C8" s="20">
+      <c r="C8" s="19">
         <v>42850</v>
       </c>
       <c r="D8" s="6" t="s">
@@ -1280,11 +1285,11 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="2:25" ht="16" customHeight="1">
+    <row r="9" spans="2:25" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="5">
         <v>5</v>
       </c>
-      <c r="C9" s="19">
+      <c r="C9" s="18">
         <v>42850</v>
       </c>
       <c r="D9" s="5" t="s">
@@ -1348,11 +1353,11 @@
       </c>
       <c r="Y9" s="1"/>
     </row>
-    <row r="10" spans="2:25" ht="16" customHeight="1">
+    <row r="10" spans="2:25" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="6">
         <v>6</v>
       </c>
-      <c r="C10" s="20">
+      <c r="C10" s="19">
         <v>42850</v>
       </c>
       <c r="D10" s="6" t="s">
@@ -1415,11 +1420,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:25" ht="16" customHeight="1">
+    <row r="11" spans="2:25" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="5">
         <v>7</v>
       </c>
-      <c r="C11" s="19">
+      <c r="C11" s="18">
         <v>42851</v>
       </c>
       <c r="D11" s="5" t="s">
@@ -1483,11 +1488,11 @@
       </c>
       <c r="Y11" s="1"/>
     </row>
-    <row r="12" spans="2:25" ht="16" customHeight="1">
+    <row r="12" spans="2:25" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="6">
         <v>8</v>
       </c>
-      <c r="C12" s="20">
+      <c r="C12" s="19">
         <v>42851</v>
       </c>
       <c r="D12" s="6" t="s">
@@ -1550,11 +1555,11 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="2:25" ht="16" customHeight="1">
+    <row r="13" spans="2:25" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="5">
         <v>9</v>
       </c>
-      <c r="C13" s="19">
+      <c r="C13" s="18">
         <v>42851</v>
       </c>
       <c r="D13" s="5" t="s">
@@ -1618,11 +1623,11 @@
       </c>
       <c r="Y13" s="1"/>
     </row>
-    <row r="14" spans="2:25" ht="16" customHeight="1">
+    <row r="14" spans="2:25" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="6">
         <v>10</v>
       </c>
-      <c r="C14" s="20">
+      <c r="C14" s="19">
         <v>42852</v>
       </c>
       <c r="D14" s="6" t="s">
@@ -1685,11 +1690,11 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="2:25" ht="16" customHeight="1">
+    <row r="15" spans="2:25" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="5">
         <v>11</v>
       </c>
-      <c r="C15" s="19">
+      <c r="C15" s="18">
         <v>42852</v>
       </c>
       <c r="D15" s="5" t="s">
@@ -1753,67 +1758,67 @@
       </c>
       <c r="Y15" s="1"/>
     </row>
-    <row r="16" spans="2:25" ht="16" customHeight="1">
+    <row r="16" spans="2:25" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="8">
         <v>12</v>
       </c>
-      <c r="C16" s="21"/>
+      <c r="C16" s="20"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
-      <c r="H16" s="17">
+      <c r="H16" s="16">
         <v>3</v>
       </c>
-      <c r="I16" s="17">
+      <c r="I16" s="16">
         <v>2</v>
       </c>
-      <c r="J16" s="17">
+      <c r="J16" s="16">
         <v>1</v>
       </c>
       <c r="K16" s="15"/>
       <c r="L16" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="M16" s="18">
-        <v>60</v>
-      </c>
-      <c r="N16" s="18">
-        <v>60</v>
-      </c>
-      <c r="O16" s="18">
-        <v>60</v>
-      </c>
-      <c r="P16" s="18">
-        <v>60</v>
-      </c>
-      <c r="Q16" s="18">
-        <v>0</v>
-      </c>
-      <c r="R16" s="18">
-        <v>0</v>
-      </c>
-      <c r="S16" s="18">
-        <v>60</v>
-      </c>
-      <c r="T16" s="18">
-        <v>60</v>
-      </c>
-      <c r="U16" s="18">
-        <v>60</v>
-      </c>
-      <c r="V16" s="18">
-        <v>60</v>
-      </c>
-      <c r="W16" s="18">
-        <v>0</v>
-      </c>
-      <c r="X16" s="18">
+      <c r="M16" s="17">
+        <v>60</v>
+      </c>
+      <c r="N16" s="17">
+        <v>60</v>
+      </c>
+      <c r="O16" s="17">
+        <v>60</v>
+      </c>
+      <c r="P16" s="17">
+        <v>60</v>
+      </c>
+      <c r="Q16" s="17">
+        <v>0</v>
+      </c>
+      <c r="R16" s="17">
+        <v>0</v>
+      </c>
+      <c r="S16" s="17">
+        <v>60</v>
+      </c>
+      <c r="T16" s="17">
+        <v>60</v>
+      </c>
+      <c r="U16" s="17">
+        <v>60</v>
+      </c>
+      <c r="V16" s="17">
+        <v>60</v>
+      </c>
+      <c r="W16" s="17">
+        <v>0</v>
+      </c>
+      <c r="X16" s="17">
         <v>0</v>
       </c>
       <c r="Y16" s="7"/>
     </row>
-    <row r="17" spans="2:25" ht="16" customHeight="1">
+    <row r="17" spans="2:25" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="5">
         <v>13</v>
       </c>
@@ -1867,7 +1872,7 @@
       </c>
       <c r="Y17" s="1"/>
     </row>
-    <row r="18" spans="2:25" ht="16" customHeight="1">
+    <row r="18" spans="2:25" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="6">
         <v>14</v>
       </c>
@@ -1920,7 +1925,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="2:25" ht="16" customHeight="1">
+    <row r="19" spans="2:25" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="5">
         <v>15</v>
       </c>
@@ -1974,7 +1979,7 @@
       </c>
       <c r="Y19" s="1"/>
     </row>
-    <row r="20" spans="2:25" ht="16" customHeight="1">
+    <row r="20" spans="2:25" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="6">
         <v>16</v>
       </c>
@@ -2027,7 +2032,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="2:25" ht="16" customHeight="1">
+    <row r="21" spans="2:25" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="5">
         <v>17</v>
       </c>
@@ -2081,7 +2086,7 @@
       </c>
       <c r="Y21" s="1"/>
     </row>
-    <row r="22" spans="2:25" ht="16" customHeight="1">
+    <row r="22" spans="2:25" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="8">
         <v>18</v>
       </c>
@@ -2090,52 +2095,52 @@
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="17"/>
-      <c r="J22" s="17"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="16"/>
       <c r="K22" s="15"/>
       <c r="L22" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="M22" s="18">
-        <v>60</v>
-      </c>
-      <c r="N22" s="18">
-        <v>60</v>
-      </c>
-      <c r="O22" s="18">
-        <v>60</v>
-      </c>
-      <c r="P22" s="18">
-        <v>60</v>
-      </c>
-      <c r="Q22" s="18">
-        <v>60</v>
-      </c>
-      <c r="R22" s="18">
-        <v>60</v>
-      </c>
-      <c r="S22" s="18">
-        <v>60</v>
-      </c>
-      <c r="T22" s="18">
-        <v>60</v>
-      </c>
-      <c r="U22" s="18">
-        <v>0</v>
-      </c>
-      <c r="V22" s="18">
-        <v>0</v>
-      </c>
-      <c r="W22" s="18">
-        <v>0</v>
-      </c>
-      <c r="X22" s="18">
+      <c r="M22" s="17">
+        <v>60</v>
+      </c>
+      <c r="N22" s="17">
+        <v>60</v>
+      </c>
+      <c r="O22" s="17">
+        <v>60</v>
+      </c>
+      <c r="P22" s="17">
+        <v>60</v>
+      </c>
+      <c r="Q22" s="17">
+        <v>60</v>
+      </c>
+      <c r="R22" s="17">
+        <v>60</v>
+      </c>
+      <c r="S22" s="17">
+        <v>60</v>
+      </c>
+      <c r="T22" s="17">
+        <v>60</v>
+      </c>
+      <c r="U22" s="17">
+        <v>0</v>
+      </c>
+      <c r="V22" s="17">
+        <v>0</v>
+      </c>
+      <c r="W22" s="17">
+        <v>0</v>
+      </c>
+      <c r="X22" s="17">
         <v>0</v>
       </c>
       <c r="Y22" s="7"/>
     </row>
-    <row r="23" spans="2:25" ht="16" customHeight="1">
+    <row r="23" spans="2:25" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="5">
         <v>19</v>
       </c>
@@ -2189,7 +2194,7 @@
       </c>
       <c r="Y23" s="1"/>
     </row>
-    <row r="24" spans="2:25" ht="16" customHeight="1">
+    <row r="24" spans="2:25" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="6">
         <v>20</v>
       </c>
@@ -2242,7 +2247,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="2:25" ht="16" customHeight="1">
+    <row r="25" spans="2:25" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="5">
         <v>21</v>
       </c>
@@ -2296,7 +2301,7 @@
       </c>
       <c r="Y25" s="1"/>
     </row>
-    <row r="26" spans="2:25" ht="16" customHeight="1">
+    <row r="26" spans="2:25" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="6">
         <v>22</v>
       </c>
@@ -2349,7 +2354,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="2:25" ht="16" customHeight="1">
+    <row r="27" spans="2:25" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="5">
         <v>23</v>
       </c>
@@ -2403,7 +2408,7 @@
       </c>
       <c r="Y27" s="1"/>
     </row>
-    <row r="28" spans="2:25" ht="16" customHeight="1">
+    <row r="28" spans="2:25" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="8">
         <v>24</v>
       </c>

</xml_diff>

<commit_message>
Session Info after Cancelation
Updated Session info sheet after Tuesday morning cancelation
</commit_message>
<xml_diff>
--- a/docs/Session Info.xlsx
+++ b/docs/Session Info.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1820" windowWidth="25600" windowHeight="16440" tabRatio="500"/>
+    <workbookView xWindow="-80" yWindow="-460" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$1:$Z$28</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$1:$Z$29</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="39">
   <si>
     <t>Pressure</t>
   </si>
@@ -124,6 +124,21 @@
   </si>
   <si>
     <t>redo</t>
+  </si>
+  <si>
+    <t>15 - fail</t>
+  </si>
+  <si>
+    <t>Only 11 showed up. 6 no shows.</t>
+  </si>
+  <si>
+    <t>1 - redo</t>
+  </si>
+  <si>
+    <t>2 - redo</t>
+  </si>
+  <si>
+    <t>3 - redo</t>
   </si>
 </sst>
 </file>
@@ -168,7 +183,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -193,8 +208,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -251,19 +272,8 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="71">
+  <cellStyleXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -335,8 +345,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -395,10 +423,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="71">
+  <cellStyles count="89">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -434,6 +481,15 @@
     <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -469,6 +525,15 @@
     <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -803,10 +868,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:AA28"/>
+  <dimension ref="B1:AA37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA21" sqref="AA21"/>
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -823,7 +888,7 @@
     <col min="13" max="13" width="1.83203125" customWidth="1"/>
     <col min="14" max="14" width="10" customWidth="1"/>
     <col min="15" max="26" width="3.5" customWidth="1"/>
-    <col min="27" max="27" width="64.83203125" customWidth="1"/>
+    <col min="27" max="27" width="28" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:27" ht="16" customHeight="1">
@@ -1251,7 +1316,9 @@
       <c r="H7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="5"/>
+      <c r="I7" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="J7" s="9">
         <v>1</v>
       </c>
@@ -1325,7 +1392,9 @@
       <c r="H8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I8" s="6"/>
+      <c r="I8" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="J8" s="10">
         <v>1</v>
       </c>
@@ -1398,7 +1467,9 @@
       <c r="H9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I9" s="5"/>
+      <c r="I9" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="J9" s="9">
         <v>2</v>
       </c>
@@ -1472,7 +1543,9 @@
       <c r="H10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I10" s="6"/>
+      <c r="I10" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="J10" s="10">
         <v>2</v>
       </c>
@@ -1545,7 +1618,9 @@
       <c r="H11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I11" s="5"/>
+      <c r="I11" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="J11" s="9">
         <v>2</v>
       </c>
@@ -1619,7 +1694,9 @@
       <c r="H12" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I12" s="6"/>
+      <c r="I12" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="J12" s="10">
         <v>2</v>
       </c>
@@ -1692,7 +1769,9 @@
       <c r="H13" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I13" s="5"/>
+      <c r="I13" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="J13" s="9">
         <v>1</v>
       </c>
@@ -1766,7 +1845,9 @@
       <c r="H14" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I14" s="6"/>
+      <c r="I14" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="J14" s="10">
         <v>1</v>
       </c>
@@ -1839,7 +1920,9 @@
       <c r="H15" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I15" s="5"/>
+      <c r="I15" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="J15" s="9">
         <v>3</v>
       </c>
@@ -1913,7 +1996,9 @@
       <c r="H16" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="8"/>
+      <c r="I16" s="8" t="s">
+        <v>23</v>
+      </c>
       <c r="J16" s="16">
         <v>3</v>
       </c>
@@ -1987,7 +2072,9 @@
       <c r="H17" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I17" s="5"/>
+      <c r="I17" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="J17" s="9">
         <v>1</v>
       </c>
@@ -2061,7 +2148,9 @@
       <c r="H18" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I18" s="6"/>
+      <c r="I18" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="J18" s="10">
         <v>3</v>
       </c>
@@ -2113,682 +2202,698 @@
       </c>
     </row>
     <row r="19" spans="2:27" ht="16" customHeight="1">
-      <c r="B19" s="5">
+      <c r="B19" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="31">
+        <v>42857</v>
+      </c>
+      <c r="E19" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="G19" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="H19" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="I19" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="J19" s="32">
+        <v>2</v>
+      </c>
+      <c r="K19" s="32">
+        <v>1</v>
+      </c>
+      <c r="L19" s="32">
+        <v>3</v>
+      </c>
+      <c r="M19" s="33"/>
+      <c r="N19" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="O19" s="34">
+        <v>60</v>
+      </c>
+      <c r="P19" s="34">
+        <v>60</v>
+      </c>
+      <c r="Q19" s="34">
+        <v>60</v>
+      </c>
+      <c r="R19" s="34">
+        <v>60</v>
+      </c>
+      <c r="S19" s="34">
+        <v>0</v>
+      </c>
+      <c r="T19" s="34">
+        <v>0</v>
+      </c>
+      <c r="U19" s="34">
+        <v>0</v>
+      </c>
+      <c r="V19" s="34">
+        <v>0</v>
+      </c>
+      <c r="W19" s="34">
+        <v>60</v>
+      </c>
+      <c r="X19" s="34">
+        <v>60</v>
+      </c>
+      <c r="Y19" s="34">
+        <v>60</v>
+      </c>
+      <c r="Z19" s="34">
+        <v>60</v>
+      </c>
+      <c r="AA19" s="34" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="2:27" ht="16" customHeight="1">
+      <c r="B20" s="5">
         <v>15</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C20" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="18">
+      <c r="D20" s="18">
         <v>42857</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="E20" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J20" s="9">
+        <v>2</v>
+      </c>
+      <c r="K20" s="9">
+        <v>1</v>
+      </c>
+      <c r="L20" s="9">
+        <v>3</v>
+      </c>
+      <c r="M20" s="13"/>
+      <c r="N20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O20" s="1">
+        <v>60</v>
+      </c>
+      <c r="P20" s="1">
+        <v>60</v>
+      </c>
+      <c r="Q20" s="1">
+        <v>60</v>
+      </c>
+      <c r="R20" s="1">
+        <v>60</v>
+      </c>
+      <c r="S20" s="1">
+        <v>0</v>
+      </c>
+      <c r="T20" s="1">
+        <v>0</v>
+      </c>
+      <c r="U20" s="1">
+        <v>0</v>
+      </c>
+      <c r="V20" s="1">
+        <v>0</v>
+      </c>
+      <c r="W20" s="1">
+        <v>60</v>
+      </c>
+      <c r="X20" s="1">
+        <v>60</v>
+      </c>
+      <c r="Y20" s="1">
+        <v>60</v>
+      </c>
+      <c r="Z20" s="1">
+        <v>60</v>
+      </c>
+      <c r="AA20" s="1"/>
+    </row>
+    <row r="21" spans="2:27" ht="16" customHeight="1">
+      <c r="B21" s="6">
+        <v>16</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="19">
+        <v>42857</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I21" s="6"/>
+      <c r="J21">
+        <v>3</v>
+      </c>
+      <c r="K21">
+        <v>2</v>
+      </c>
+      <c r="L21">
+        <v>1</v>
+      </c>
+      <c r="M21" s="14"/>
+      <c r="N21" t="s">
+        <v>1</v>
+      </c>
+      <c r="O21" s="2">
+        <v>60</v>
+      </c>
+      <c r="P21" s="2">
+        <v>60</v>
+      </c>
+      <c r="Q21" s="2">
+        <v>60</v>
+      </c>
+      <c r="R21" s="2">
+        <v>60</v>
+      </c>
+      <c r="S21" s="2">
+        <v>0</v>
+      </c>
+      <c r="T21" s="2">
+        <v>0</v>
+      </c>
+      <c r="U21" s="2">
+        <v>0</v>
+      </c>
+      <c r="V21" s="2">
+        <v>0</v>
+      </c>
+      <c r="W21" s="2">
+        <v>60</v>
+      </c>
+      <c r="X21" s="2">
+        <v>60</v>
+      </c>
+      <c r="Y21" s="2">
+        <v>60</v>
+      </c>
+      <c r="Z21" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="2:27" ht="16" customHeight="1">
+      <c r="B22" s="5">
+        <v>17</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="18">
+        <v>42858</v>
+      </c>
+      <c r="E22" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="F22" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="G22" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H19" s="5" t="s">
+      <c r="H22" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I19" s="5"/>
-      <c r="J19" s="9">
+      <c r="I22" s="5"/>
+      <c r="J22" s="9">
         <v>2</v>
       </c>
-      <c r="K19" s="9">
-        <v>1</v>
-      </c>
-      <c r="L19" s="9">
+      <c r="K22" s="9">
         <v>3</v>
       </c>
-      <c r="M19" s="13"/>
-      <c r="N19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O19" s="1">
-        <v>60</v>
-      </c>
-      <c r="P19" s="1">
-        <v>60</v>
-      </c>
-      <c r="Q19" s="1">
-        <v>60</v>
-      </c>
-      <c r="R19" s="1">
-        <v>60</v>
-      </c>
-      <c r="S19" s="1">
-        <v>0</v>
-      </c>
-      <c r="T19" s="1">
-        <v>0</v>
-      </c>
-      <c r="U19" s="1">
-        <v>0</v>
-      </c>
-      <c r="V19" s="1">
-        <v>0</v>
-      </c>
-      <c r="W19" s="1">
-        <v>60</v>
-      </c>
-      <c r="X19" s="1">
-        <v>60</v>
-      </c>
-      <c r="Y19" s="1">
-        <v>60</v>
-      </c>
-      <c r="Z19" s="1">
-        <v>60</v>
-      </c>
-      <c r="AA19" s="1"/>
-    </row>
-    <row r="20" spans="2:27" ht="16" customHeight="1">
-      <c r="B20" s="6">
-        <v>16</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D20" s="19">
-        <v>42857</v>
-      </c>
-      <c r="E20" s="6" t="s">
+      <c r="L22" s="9">
+        <v>1</v>
+      </c>
+      <c r="M22" s="13"/>
+      <c r="N22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O22" s="1">
+        <v>60</v>
+      </c>
+      <c r="P22" s="1">
+        <v>60</v>
+      </c>
+      <c r="Q22" s="1">
+        <v>60</v>
+      </c>
+      <c r="R22" s="1">
+        <v>60</v>
+      </c>
+      <c r="S22" s="1">
+        <v>60</v>
+      </c>
+      <c r="T22" s="1">
+        <v>60</v>
+      </c>
+      <c r="U22" s="1">
+        <v>60</v>
+      </c>
+      <c r="V22" s="1">
+        <v>60</v>
+      </c>
+      <c r="W22" s="1">
+        <v>0</v>
+      </c>
+      <c r="X22" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y22" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z22" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA22" s="1"/>
+    </row>
+    <row r="23" spans="2:27" ht="16" customHeight="1">
+      <c r="B23" s="8">
+        <v>18</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="20">
+        <v>42858</v>
+      </c>
+      <c r="E23" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="F23" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G20" s="6" t="s">
+      <c r="G23" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H20" s="6" t="s">
+      <c r="H23" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="I20" s="6"/>
-      <c r="J20" s="10">
-        <v>1</v>
-      </c>
-      <c r="K20" s="10">
+      <c r="I23" s="8"/>
+      <c r="J23" s="16">
+        <v>1</v>
+      </c>
+      <c r="K23" s="16">
         <v>3</v>
       </c>
-      <c r="L20" s="10">
+      <c r="L23" s="16">
         <v>2</v>
       </c>
-      <c r="M20" s="14"/>
-      <c r="N20" t="s">
-        <v>1</v>
-      </c>
-      <c r="O20" s="2">
-        <v>60</v>
-      </c>
-      <c r="P20" s="2">
-        <v>60</v>
-      </c>
-      <c r="Q20" s="2">
-        <v>60</v>
-      </c>
-      <c r="R20" s="2">
-        <v>60</v>
-      </c>
-      <c r="S20" s="2">
-        <v>0</v>
-      </c>
-      <c r="T20" s="2">
-        <v>0</v>
-      </c>
-      <c r="U20" s="2">
-        <v>0</v>
-      </c>
-      <c r="V20" s="2">
-        <v>0</v>
-      </c>
-      <c r="W20" s="2">
-        <v>60</v>
-      </c>
-      <c r="X20" s="2">
-        <v>60</v>
-      </c>
-      <c r="Y20" s="2">
-        <v>60</v>
-      </c>
-      <c r="Z20" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="21" spans="2:27" ht="16" customHeight="1">
-      <c r="B21" s="5">
-        <v>17</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D21" s="18">
-        <v>42857</v>
-      </c>
-      <c r="E21" s="5" t="s">
+      <c r="M23" s="15"/>
+      <c r="N23" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="O23" s="17">
+        <v>60</v>
+      </c>
+      <c r="P23" s="17">
+        <v>60</v>
+      </c>
+      <c r="Q23" s="17">
+        <v>60</v>
+      </c>
+      <c r="R23" s="17">
+        <v>60</v>
+      </c>
+      <c r="S23" s="17">
+        <v>60</v>
+      </c>
+      <c r="T23" s="17">
+        <v>60</v>
+      </c>
+      <c r="U23" s="17">
+        <v>60</v>
+      </c>
+      <c r="V23" s="17">
+        <v>60</v>
+      </c>
+      <c r="W23" s="17">
+        <v>0</v>
+      </c>
+      <c r="X23" s="17">
+        <v>0</v>
+      </c>
+      <c r="Y23" s="17">
+        <v>0</v>
+      </c>
+      <c r="Z23" s="17">
+        <v>0</v>
+      </c>
+      <c r="AA23" s="7"/>
+    </row>
+    <row r="24" spans="2:27" ht="16" customHeight="1">
+      <c r="B24" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" s="18">
+        <v>42858</v>
+      </c>
+      <c r="E24" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F21" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G21" s="5" t="s">
+      <c r="F24" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G24" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H21" s="5" t="s">
+      <c r="H24" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I21" s="5"/>
-      <c r="J21" s="9">
+      <c r="I24" s="5"/>
+      <c r="J24" s="9">
+        <v>1</v>
+      </c>
+      <c r="K24" s="9">
+        <v>2</v>
+      </c>
+      <c r="L24" s="9">
         <v>3</v>
       </c>
-      <c r="K21" s="9">
+      <c r="M24" s="13"/>
+      <c r="N24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O24" s="1">
+        <v>60</v>
+      </c>
+      <c r="P24" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="3">
+        <v>60</v>
+      </c>
+      <c r="R24" s="1">
+        <v>60</v>
+      </c>
+      <c r="S24" s="1">
+        <v>0</v>
+      </c>
+      <c r="T24" s="3">
+        <v>60</v>
+      </c>
+      <c r="U24" s="1">
+        <v>60</v>
+      </c>
+      <c r="V24" s="1">
+        <v>0</v>
+      </c>
+      <c r="W24" s="3">
+        <v>60</v>
+      </c>
+      <c r="X24" s="1">
+        <v>60</v>
+      </c>
+      <c r="Y24" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z24" s="3">
+        <v>60</v>
+      </c>
+      <c r="AA24" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="2:27" ht="16" customHeight="1">
+      <c r="B25" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25" s="19">
+        <v>42859</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I25" s="6"/>
+      <c r="J25" s="10">
+        <v>3</v>
+      </c>
+      <c r="K25" s="10">
         <v>2</v>
       </c>
-      <c r="L21" s="9">
-        <v>1</v>
-      </c>
-      <c r="M21" s="13"/>
-      <c r="N21" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O21" s="1">
-        <v>60</v>
-      </c>
-      <c r="P21" s="1">
-        <v>60</v>
-      </c>
-      <c r="Q21" s="1">
-        <v>60</v>
-      </c>
-      <c r="R21" s="1">
-        <v>60</v>
-      </c>
-      <c r="S21" s="1">
-        <v>60</v>
-      </c>
-      <c r="T21" s="1">
-        <v>60</v>
-      </c>
-      <c r="U21" s="1">
-        <v>60</v>
-      </c>
-      <c r="V21" s="1">
-        <v>60</v>
-      </c>
-      <c r="W21" s="1">
-        <v>0</v>
-      </c>
-      <c r="X21" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y21" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z21" s="1">
-        <v>0</v>
-      </c>
-      <c r="AA21" s="1"/>
-    </row>
-    <row r="22" spans="2:27" ht="16" customHeight="1">
-      <c r="B22" s="8">
-        <v>18</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D22" s="20">
-        <v>42858</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F22" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="G22" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="H22" s="8" t="s">
+      <c r="L25" s="10">
+        <v>1</v>
+      </c>
+      <c r="M25" s="14"/>
+      <c r="N25" t="s">
+        <v>0</v>
+      </c>
+      <c r="O25" s="2">
+        <v>60</v>
+      </c>
+      <c r="P25" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="2">
+        <v>60</v>
+      </c>
+      <c r="R25" s="2">
+        <v>0</v>
+      </c>
+      <c r="S25" s="2">
+        <v>60</v>
+      </c>
+      <c r="T25" s="2">
+        <v>60</v>
+      </c>
+      <c r="U25" s="2">
+        <v>0</v>
+      </c>
+      <c r="V25" s="2">
+        <v>60</v>
+      </c>
+      <c r="W25" s="2">
+        <v>60</v>
+      </c>
+      <c r="X25" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y25" s="2">
+        <v>60</v>
+      </c>
+      <c r="Z25" s="2">
+        <v>60</v>
+      </c>
+      <c r="AA25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="2:27" ht="16" customHeight="1">
+      <c r="B26" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26" s="18">
+        <v>42859</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I22" s="8"/>
-      <c r="J22" s="16">
+      <c r="I26" s="5"/>
+      <c r="J26" s="9">
         <v>3</v>
       </c>
-      <c r="K22" s="16">
+      <c r="K26" s="9">
+        <v>1</v>
+      </c>
+      <c r="L26" s="9">
         <v>2</v>
       </c>
-      <c r="L22" s="16">
-        <v>1</v>
-      </c>
-      <c r="M22" s="15"/>
-      <c r="N22" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="O22" s="17">
-        <v>60</v>
-      </c>
-      <c r="P22" s="17">
-        <v>60</v>
-      </c>
-      <c r="Q22" s="17">
-        <v>60</v>
-      </c>
-      <c r="R22" s="17">
-        <v>60</v>
-      </c>
-      <c r="S22" s="17">
-        <v>60</v>
-      </c>
-      <c r="T22" s="17">
-        <v>60</v>
-      </c>
-      <c r="U22" s="17">
-        <v>60</v>
-      </c>
-      <c r="V22" s="17">
-        <v>60</v>
-      </c>
-      <c r="W22" s="17">
-        <v>0</v>
-      </c>
-      <c r="X22" s="17">
-        <v>0</v>
-      </c>
-      <c r="Y22" s="17">
-        <v>0</v>
-      </c>
-      <c r="Z22" s="17">
-        <v>0</v>
-      </c>
-      <c r="AA22" s="7" t="s">
+      <c r="M26" s="13"/>
+      <c r="N26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O26" s="1">
+        <v>60</v>
+      </c>
+      <c r="P26" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="3">
+        <v>60</v>
+      </c>
+      <c r="R26" s="1">
+        <v>0</v>
+      </c>
+      <c r="S26" s="1">
+        <v>60</v>
+      </c>
+      <c r="T26" s="3">
+        <v>60</v>
+      </c>
+      <c r="U26" s="1">
+        <v>0</v>
+      </c>
+      <c r="V26" s="1">
+        <v>60</v>
+      </c>
+      <c r="W26" s="3">
+        <v>60</v>
+      </c>
+      <c r="X26" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y26" s="1">
+        <v>60</v>
+      </c>
+      <c r="Z26" s="3">
+        <v>60</v>
+      </c>
+      <c r="AA26" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="2:27" ht="16" customHeight="1">
-      <c r="B23" s="5">
-        <v>19</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D23" s="18">
-        <v>42858</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G23" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H23" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="I23" s="5"/>
-      <c r="J23" s="9">
-        <v>2</v>
-      </c>
-      <c r="K23" s="9">
-        <v>3</v>
-      </c>
-      <c r="L23" s="9">
-        <v>1</v>
-      </c>
-      <c r="M23" s="13"/>
-      <c r="N23" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O23" s="1">
-        <v>0</v>
-      </c>
-      <c r="P23" s="1">
-        <v>60</v>
-      </c>
-      <c r="Q23" s="1">
-        <v>60</v>
-      </c>
-      <c r="R23" s="1">
-        <v>0</v>
-      </c>
-      <c r="S23" s="1">
-        <v>60</v>
-      </c>
-      <c r="T23" s="1">
-        <v>60</v>
-      </c>
-      <c r="U23" s="1">
-        <v>0</v>
-      </c>
-      <c r="V23" s="1">
-        <v>60</v>
-      </c>
-      <c r="W23" s="1">
-        <v>60</v>
-      </c>
-      <c r="X23" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y23" s="1">
-        <v>60</v>
-      </c>
-      <c r="Z23" s="1">
-        <v>60</v>
-      </c>
-      <c r="AA23" s="1"/>
-    </row>
-    <row r="24" spans="2:27" ht="16" customHeight="1">
-      <c r="B24" s="6">
-        <v>20</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D24" s="19">
-        <v>42858</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G24" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H24" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I24" s="6"/>
-      <c r="J24" s="10">
-        <v>1</v>
-      </c>
-      <c r="K24" s="10">
-        <v>2</v>
-      </c>
-      <c r="L24" s="10">
-        <v>3</v>
-      </c>
-      <c r="M24" s="14"/>
-      <c r="N24" t="s">
-        <v>1</v>
-      </c>
-      <c r="O24" s="2">
-        <v>0</v>
-      </c>
-      <c r="P24" s="2">
-        <v>60</v>
-      </c>
-      <c r="Q24" s="2">
-        <v>60</v>
-      </c>
-      <c r="R24" s="2">
-        <v>0</v>
-      </c>
-      <c r="S24" s="2">
-        <v>60</v>
-      </c>
-      <c r="T24" s="2">
-        <v>60</v>
-      </c>
-      <c r="U24" s="2">
-        <v>0</v>
-      </c>
-      <c r="V24" s="2">
-        <v>60</v>
-      </c>
-      <c r="W24" s="2">
-        <v>60</v>
-      </c>
-      <c r="X24" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y24" s="2">
-        <v>60</v>
-      </c>
-      <c r="Z24" s="2">
-        <v>60</v>
-      </c>
-      <c r="AA24" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="25" spans="2:27" ht="16" customHeight="1">
-      <c r="B25" s="5">
-        <v>21</v>
-      </c>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="9">
-        <v>3</v>
-      </c>
-      <c r="K25" s="9">
-        <v>1</v>
-      </c>
-      <c r="L25" s="9">
-        <v>2</v>
-      </c>
-      <c r="M25" s="13"/>
-      <c r="N25" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O25" s="1">
-        <v>60</v>
-      </c>
-      <c r="P25" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q25" s="3">
-        <v>60</v>
-      </c>
-      <c r="R25" s="1">
-        <v>60</v>
-      </c>
-      <c r="S25" s="1">
-        <v>0</v>
-      </c>
-      <c r="T25" s="3">
-        <v>60</v>
-      </c>
-      <c r="U25" s="1">
-        <v>60</v>
-      </c>
-      <c r="V25" s="1">
-        <v>0</v>
-      </c>
-      <c r="W25" s="3">
-        <v>60</v>
-      </c>
-      <c r="X25" s="1">
-        <v>60</v>
-      </c>
-      <c r="Y25" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z25" s="3">
-        <v>60</v>
-      </c>
-      <c r="AA25" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="26" spans="2:27" ht="16" customHeight="1">
-      <c r="B26" s="6">
-        <v>22</v>
-      </c>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="6"/>
-      <c r="K26" s="6"/>
-      <c r="L26" s="6"/>
-      <c r="M26" s="14"/>
-      <c r="N26" t="s">
-        <v>1</v>
-      </c>
-      <c r="O26" s="2">
-        <v>60</v>
-      </c>
-      <c r="P26" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q26" s="4">
-        <v>60</v>
-      </c>
-      <c r="R26" s="2">
-        <v>60</v>
-      </c>
-      <c r="S26" s="2">
-        <v>0</v>
-      </c>
-      <c r="T26" s="4">
-        <v>60</v>
-      </c>
-      <c r="U26" s="2">
-        <v>60</v>
-      </c>
-      <c r="V26" s="2">
-        <v>0</v>
-      </c>
-      <c r="W26" s="4">
-        <v>60</v>
-      </c>
-      <c r="X26" s="2">
-        <v>60</v>
-      </c>
-      <c r="Y26" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z26" s="4">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="27" spans="2:27" ht="16" customHeight="1">
-      <c r="B27" s="5">
-        <v>23</v>
-      </c>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
-      <c r="I27" s="5"/>
-      <c r="J27" s="5"/>
-      <c r="K27" s="5"/>
-      <c r="L27" s="5"/>
-      <c r="M27" s="13"/>
-      <c r="N27" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O27" s="3">
-        <v>60</v>
-      </c>
-      <c r="P27" s="1">
-        <v>60</v>
-      </c>
-      <c r="Q27" s="1">
-        <v>0</v>
-      </c>
-      <c r="R27" s="3">
-        <v>60</v>
-      </c>
-      <c r="S27" s="3">
-        <v>60</v>
-      </c>
-      <c r="T27" s="1">
-        <v>0</v>
-      </c>
-      <c r="U27" s="3">
-        <v>60</v>
-      </c>
-      <c r="V27" s="3">
-        <v>60</v>
-      </c>
-      <c r="W27" s="1">
-        <v>0</v>
-      </c>
-      <c r="X27" s="3">
-        <v>60</v>
-      </c>
-      <c r="Y27" s="3">
-        <v>60</v>
-      </c>
-      <c r="Z27" s="1">
-        <v>0</v>
-      </c>
-      <c r="AA27" s="1"/>
-    </row>
-    <row r="28" spans="2:27" ht="16" customHeight="1">
-      <c r="B28" s="8">
-        <v>24</v>
-      </c>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="8"/>
-      <c r="L28" s="8"/>
-      <c r="M28" s="15"/>
-      <c r="N28" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="O28" s="31">
-        <v>60</v>
-      </c>
-      <c r="P28" s="17">
-        <v>60</v>
-      </c>
-      <c r="Q28" s="17">
-        <v>0</v>
-      </c>
-      <c r="R28" s="31">
-        <v>60</v>
-      </c>
-      <c r="S28" s="31">
-        <v>60</v>
-      </c>
-      <c r="T28" s="17">
-        <v>0</v>
-      </c>
-      <c r="U28" s="31">
-        <v>60</v>
-      </c>
-      <c r="V28" s="31">
-        <v>60</v>
-      </c>
-      <c r="W28" s="17">
-        <v>0</v>
-      </c>
-      <c r="X28" s="31">
-        <v>60</v>
-      </c>
-      <c r="Y28" s="31">
-        <v>60</v>
-      </c>
-      <c r="Z28" s="17">
-        <v>0</v>
-      </c>
-      <c r="AA28" s="7"/>
+    <row r="27" spans="2:27" s="37" customFormat="1" ht="16" customHeight="1">
+      <c r="B27" s="36"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="36"/>
+      <c r="J27" s="36"/>
+      <c r="K27" s="36"/>
+      <c r="L27" s="36"/>
+      <c r="M27" s="36"/>
+      <c r="Q27" s="38"/>
+      <c r="T27" s="38"/>
+      <c r="W27" s="38"/>
+      <c r="Z27" s="38"/>
+    </row>
+    <row r="28" spans="2:27" s="37" customFormat="1" ht="16" customHeight="1">
+      <c r="B28" s="36"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="36"/>
+      <c r="G28" s="36"/>
+      <c r="H28" s="36"/>
+      <c r="I28" s="36"/>
+      <c r="J28" s="36"/>
+      <c r="K28" s="36"/>
+      <c r="L28" s="36"/>
+      <c r="M28" s="36"/>
+      <c r="O28" s="38"/>
+      <c r="R28" s="38"/>
+      <c r="S28" s="38"/>
+      <c r="U28" s="38"/>
+      <c r="V28" s="38"/>
+      <c r="X28" s="38"/>
+      <c r="Y28" s="38"/>
+    </row>
+    <row r="29" spans="2:27" s="37" customFormat="1" ht="16" customHeight="1">
+      <c r="B29" s="36"/>
+      <c r="C29" s="36"/>
+      <c r="D29" s="36"/>
+      <c r="E29" s="36"/>
+      <c r="F29" s="36"/>
+      <c r="G29" s="36"/>
+      <c r="H29" s="36"/>
+      <c r="I29" s="36"/>
+      <c r="J29" s="36"/>
+      <c r="K29" s="36"/>
+      <c r="L29" s="36"/>
+      <c r="M29" s="36"/>
+      <c r="O29" s="38"/>
+      <c r="R29" s="38"/>
+      <c r="S29" s="38"/>
+      <c r="U29" s="38"/>
+      <c r="V29" s="38"/>
+      <c r="X29" s="38"/>
+      <c r="Y29" s="38"/>
+    </row>
+    <row r="31" spans="2:27">
+      <c r="J31" s="10"/>
+      <c r="K31" s="10"/>
+      <c r="L31" s="10"/>
+    </row>
+    <row r="32" spans="2:27">
+      <c r="J32" s="10"/>
+      <c r="K32" s="10"/>
+      <c r="L32" s="10"/>
+    </row>
+    <row r="33" spans="10:12">
+      <c r="J33" s="35"/>
+      <c r="K33" s="35"/>
+      <c r="L33" s="35"/>
+    </row>
+    <row r="34" spans="10:12">
+      <c r="J34" s="35"/>
+      <c r="K34" s="35"/>
+      <c r="L34" s="35"/>
+    </row>
+    <row r="35" spans="10:12">
+      <c r="J35" s="35"/>
+      <c r="K35" s="35"/>
+      <c r="L35" s="35"/>
+    </row>
+    <row r="36" spans="10:12">
+      <c r="J36" s="35"/>
+      <c r="K36" s="35"/>
+      <c r="L36" s="35"/>
+    </row>
+    <row r="37" spans="10:12">
+      <c r="J37" s="35"/>
+      <c r="K37" s="35"/>
+      <c r="L37" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>